<commit_message>
2021 Day 5 (slow but it works)
</commit_message>
<xml_diff>
--- a/2020/Day10.xlsx
+++ b/2020/Day10.xlsx
@@ -5,18 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Financial Modelling World Cup/AoC2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Financial Modelling World Cup/Advent-of-Code-Excel/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BC6F79-130F-B140-8D72-F17746E5B1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{A698A544-30DC-0646-B24B-313790393526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
+    <workbookView xWindow="17100" yWindow="760" windowWidth="17460" windowHeight="21580" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Solutions" sheetId="1" r:id="rId1"/>
+    <sheet name="Solutions" sheetId="3" r:id="rId1"/>
     <sheet name="Workings" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="input">Workings!$A$2:$A$102</definedName>
+    <definedName name="Number1">Workings!#REF!</definedName>
+    <definedName name="Number2">Workings!#REF!</definedName>
+    <definedName name="Target">Workings!#REF!</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +40,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
@@ -47,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,6 +90,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -90,10 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,11 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344FFF3B-D6C6-1B4A-8070-5BE3B66922E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20A22F2-6DC6-9649-B622-E18762B0409B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,7 +455,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2">
+        <f>COUNTIF(Workings!C:C,1)*COUNTIF(Workings!C:C,3)</f>
+        <v>2312</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -435,12 +473,1239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8F4387-9FD6-E241-86F1-7FFD05E57526}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f>MAX(input)+3</f>
+        <v>170</v>
+      </c>
+      <c r="B1" cm="1">
+        <f t="array" ref="B1:B102">_xlfn._xlws.SORT(A1:A102)</f>
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>B1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>99</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>B2-B1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>151</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">B3-B2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>134</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>112</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>119</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>137</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>158</v>
+      </c>
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>167</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>116</v>
+      </c>
+      <c r="B16">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>117</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>62</v>
+      </c>
+      <c r="B18">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>82</v>
+      </c>
+      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>88</v>
+      </c>
+      <c r="B23">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>165</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>108</v>
+      </c>
+      <c r="B29">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>166</v>
+      </c>
+      <c r="B30">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>71</v>
+      </c>
+      <c r="B31">
+        <v>51</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>51</v>
+      </c>
+      <c r="B32">
+        <v>54</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>135</v>
+      </c>
+      <c r="B34">
+        <v>56</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>122</v>
+      </c>
+      <c r="B35">
+        <v>57</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>140</v>
+      </c>
+      <c r="B36">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>109</v>
+      </c>
+      <c r="B37">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>101</v>
+      </c>
+      <c r="B39">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>66</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>77</v>
+      </c>
+      <c r="B41">
+        <v>69</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>85</v>
+      </c>
+      <c r="B42">
+        <v>70</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>76</v>
+      </c>
+      <c r="B43">
+        <v>71</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>143</v>
+      </c>
+      <c r="B44">
+        <v>72</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>100</v>
+      </c>
+      <c r="B45">
+        <v>75</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>127</v>
+      </c>
+      <c r="B46">
+        <v>76</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>77</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>107</v>
+      </c>
+      <c r="B48">
+        <v>78</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>13</v>
+      </c>
+      <c r="B49">
+        <v>79</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>148</v>
+      </c>
+      <c r="B50">
+        <v>82</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>118</v>
+      </c>
+      <c r="B51">
+        <v>83</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>84</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>159</v>
+      </c>
+      <c r="B53">
+        <v>85</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>133</v>
+      </c>
+      <c r="B54">
+        <v>88</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>21</v>
+      </c>
+      <c r="B55">
+        <v>91</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>154</v>
+      </c>
+      <c r="B56">
+        <v>94</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>152</v>
+      </c>
+      <c r="B57">
+        <v>95</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>130</v>
+      </c>
+      <c r="B58">
+        <v>98</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>78</v>
+      </c>
+      <c r="B59">
+        <v>99</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>54</v>
+      </c>
+      <c r="B60">
+        <v>100</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>104</v>
+      </c>
+      <c r="B61">
+        <v>101</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>160</v>
+      </c>
+      <c r="B62">
+        <v>104</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>153</v>
+      </c>
+      <c r="B63">
+        <v>107</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>95</v>
+      </c>
+      <c r="B64">
+        <v>108</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>49</v>
+      </c>
+      <c r="B65">
+        <v>109</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>19</v>
+      </c>
+      <c r="B66">
+        <v>112</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>69</v>
+      </c>
+      <c r="B67">
+        <v>115</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C102" si="1">B67-B66</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>142</v>
+      </c>
+      <c r="B68">
+        <v>116</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>63</v>
+      </c>
+      <c r="B69">
+        <v>117</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>11</v>
+      </c>
+      <c r="B70">
+        <v>118</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>12</v>
+      </c>
+      <c r="B71">
+        <v>119</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>29</v>
+      </c>
+      <c r="B72">
+        <v>122</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>98</v>
+      </c>
+      <c r="B73">
+        <v>125</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>84</v>
+      </c>
+      <c r="B74">
+        <v>126</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>28</v>
+      </c>
+      <c r="B75">
+        <v>127</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>130</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>146</v>
+      </c>
+      <c r="B77">
+        <v>133</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>161</v>
+      </c>
+      <c r="B78">
+        <v>134</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>115</v>
+      </c>
+      <c r="B79">
+        <v>135</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>136</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>94</v>
+      </c>
+      <c r="B81">
+        <v>137</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>24</v>
+      </c>
+      <c r="B82">
+        <v>140</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>126</v>
+      </c>
+      <c r="B83">
+        <v>141</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>136</v>
+      </c>
+      <c r="B84">
+        <v>142</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>91</v>
+      </c>
+      <c r="B85">
+        <v>143</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>57</v>
+      </c>
+      <c r="B86">
+        <v>146</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>30</v>
+      </c>
+      <c r="B87">
+        <v>147</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>155</v>
+      </c>
+      <c r="B88">
+        <v>148</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>79</v>
+      </c>
+      <c r="B89">
+        <v>151</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>66</v>
+      </c>
+      <c r="B90">
+        <v>152</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>141</v>
+      </c>
+      <c r="B91">
+        <v>153</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>48</v>
+      </c>
+      <c r="B92">
+        <v>154</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>125</v>
+      </c>
+      <c r="B93">
+        <v>155</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>162</v>
+      </c>
+      <c r="B94">
+        <v>158</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>37</v>
+      </c>
+      <c r="B95">
+        <v>159</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>40</v>
+      </c>
+      <c r="B96">
+        <v>160</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <v>147</v>
+      </c>
+      <c r="B97">
+        <v>161</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>18</v>
+      </c>
+      <c r="B98">
+        <v>162</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>20</v>
+      </c>
+      <c r="B99">
+        <v>165</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>45</v>
+      </c>
+      <c r="B100">
+        <v>166</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>55</v>
+      </c>
+      <c r="B101">
+        <v>167</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>83</v>
+      </c>
+      <c r="B102">
+        <v>170</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>